<commit_message>
Testing alternate port scenario
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_min.xlsx
+++ b/fabrication_ports/ports_scenario_min.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1861BCD3-2551-4C76-BB64-9158E19DB770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133628C6-93CB-441D-A7DC-0D6181FFF5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41400" yWindow="13380" windowWidth="2970" windowHeight="1455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="2160" windowWidth="1980" windowHeight="970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$9:$E$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Avg Demand Scenario'!$E$10:$E$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="171">
   <si>
     <t>Port</t>
   </si>
@@ -548,6 +548,9 @@
   </si>
   <si>
     <t>USFR planned to be done in 2024</t>
+  </si>
+  <si>
+    <t>Floating date adder</t>
   </si>
 </sst>
 </file>
@@ -759,7 +762,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$10:$B$46</c:f>
+              <c:f>'Avg Demand Scenario'!$B$11:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
@@ -878,7 +881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$G$10:$G$46</c:f>
+              <c:f>'Avg Demand Scenario'!$G$11:$G$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -919,7 +922,7 @@
                   <c:v>2023</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2023</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2020</c:v>
@@ -973,10 +976,10 @@
                   <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2025</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2026</c:v>
+                  <c:v>2024</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>2031</c:v>
@@ -1017,7 +1020,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$B$10:$B$46</c:f>
+              <c:f>'Avg Demand Scenario'!$B$11:$B$47</c:f>
               <c:strCache>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
@@ -1136,7 +1139,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$L$10:$L$46</c:f>
+              <c:f>'Avg Demand Scenario'!$L$11:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -1582,7 +1585,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$I$51</c:f>
+              <c:f>'Avg Demand Scenario'!$I$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1603,7 +1606,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Avg Demand Scenario'!$H$52:$H$70</c:f>
+              <c:f>'Avg Demand Scenario'!$H$53:$H$71</c:f>
               <c:strCache>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
@@ -1665,7 +1668,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Avg Demand Scenario'!$I$52:$I$70</c:f>
+              <c:f>'Avg Demand Scenario'!$I$53:$I$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -3045,13 +3048,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>30254</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>58177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>244928</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3081,13 +3084,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>898921</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>75008</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>2458640</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>151208</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3119,7 +3122,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Shields, Matt" refreshedDate="44771.490716435183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{8520C2B9-52CF-46B0-8F6A-64DE6645DC34}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A9:L46" sheet="Avg Demand Scenario"/>
+    <worksheetSource ref="A10:L47" sheet="Avg Demand Scenario"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Component" numFmtId="0">
@@ -3739,7 +3742,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CA5F775-FB12-4A7B-98B7-3842EC7091C4}" name="PivotTable1" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="H51:I70" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="H52:I71" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -4152,10 +4155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4206,10 +4209,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>100</v>
@@ -4217,193 +4220,163 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>168</v>
+        <v>99</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>146</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>2021</v>
       </c>
-      <c r="H10">
-        <f>$D$5</f>
+      <c r="H11">
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <f>$D$3</f>
         <v>0.25</v>
       </c>
-      <c r="K10">
-        <f>ROUNDDOWN(G10+H10+I10*(1-J10),0)</f>
-        <v>2025</v>
-      </c>
-      <c r="L10">
-        <f>K10-G10</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>2023</v>
-      </c>
-      <c r="H11">
-        <f>$D$5</f>
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <f t="shared" ref="J11:J14" si="0">$D$3</f>
-        <v>0.25</v>
-      </c>
       <c r="K11">
         <f>ROUNDDOWN(G11+H11+I11*(1-J11),0)</f>
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L46" si="1">K11-G11</f>
+        <f>K11-G11</f>
         <v>4</v>
-      </c>
-      <c r="M11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G12">
+        <f>$D$4</f>
         <v>2023</v>
       </c>
       <c r="H12">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I12">
         <v>3</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J12:J15" si="0">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K46" si="2">ROUNDDOWN(G12+H12+I12*(1-J12),0)</f>
+        <f>ROUNDDOWN(G12+H12+I12*(1-J12),0)</f>
         <v>2027</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L12:L47" si="1">K12-G12</f>
         <v>4</v>
       </c>
       <c r="M12" t="s">
@@ -4412,25 +4385,26 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G13">
+        <f t="shared" ref="G13:G15" si="2">$D$4</f>
         <v>2023</v>
       </c>
       <c r="H13">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I13">
@@ -4441,7 +4415,7 @@
         <v>0.25</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K13:K47" si="3">ROUNDDOWN(G13+H13+I13*(1-J13),0)</f>
         <v>2027</v>
       </c>
       <c r="L13">
@@ -4449,31 +4423,32 @@
         <v>4</v>
       </c>
       <c r="M13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>121</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="G14">
-        <v>2024</v>
+        <f t="shared" si="2"/>
+        <v>2023</v>
       </c>
       <c r="H14">
-        <f>$D$5+$D$6</f>
-        <v>3</v>
+        <f>$D$6</f>
+        <v>2</v>
       </c>
       <c r="I14">
         <v>3</v>
@@ -4483,62 +4458,63 @@
         <v>0.25</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
-        <v>2029</v>
+        <f t="shared" si="3"/>
+        <v>2027</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="M14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
+        <v>144</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="G15">
-        <v>2021</v>
+        <f>$D$4+$D$5</f>
+        <v>2024</v>
       </c>
       <c r="H15">
-        <f>$D$5</f>
-        <v>2</v>
+        <f>$D$6+$D$7</f>
+        <v>3</v>
       </c>
       <c r="I15">
         <v>3</v>
       </c>
       <c r="J15">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
-        <v>2025</v>
+        <f t="shared" si="3"/>
+        <v>2029</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="M15" t="s">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>145</v>
@@ -4556,7 +4532,7 @@
         <v>2021</v>
       </c>
       <c r="H16">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I16">
@@ -4567,7 +4543,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="K16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2025</v>
       </c>
       <c r="L16">
@@ -4580,199 +4556,201 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G17">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H17">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17" si="3">$D$3</f>
-        <v>0.25</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K17">
-        <f t="shared" si="2"/>
-        <v>2027</v>
+        <f t="shared" si="3"/>
+        <v>2025</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="M17" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>123</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="G18">
+        <f t="shared" ref="G18" si="4">$D$4</f>
         <v>2023</v>
       </c>
       <c r="H18">
-        <f>$D$5+$D$6</f>
-        <v>3</v>
+        <f>$D$6</f>
+        <v>2</v>
       </c>
       <c r="I18">
         <v>3</v>
       </c>
       <c r="J18">
+        <f t="shared" ref="J18" si="5">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="K18" si="4">ROUNDDOWN(G18+H18+I18*(1-J18),0)</f>
+        <f t="shared" si="3"/>
+        <v>2027</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19">
+        <v>2023</v>
+      </c>
+      <c r="H19">
+        <f>$D$6+$D$7</f>
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>0.25</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="K19" si="6">ROUNDDOWN(G19+H19+I19*(1-J19),0)</f>
         <v>2028</v>
       </c>
-      <c r="L18">
-        <f t="shared" ref="L18" si="5">K18-G18</f>
+      <c r="L19">
+        <f t="shared" ref="L19" si="7">K19-G19</f>
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>24</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>2021</v>
       </c>
-      <c r="H19">
-        <f>$D$5</f>
+      <c r="H20">
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>2</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>0.8</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="2"/>
+      <c r="K20">
+        <f t="shared" si="3"/>
         <v>2023</v>
       </c>
-      <c r="L19">
+      <c r="L20">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M20" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20">
-        <v>2023</v>
-      </c>
-      <c r="H20">
-        <f>$D$5</f>
-        <v>2</v>
-      </c>
-      <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ref="J20:J22" si="6">$D$3</f>
-        <v>0.25</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="2"/>
-        <v>2026</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G21">
+        <f t="shared" ref="G21:G23" si="8">$D$4</f>
         <v>2023</v>
       </c>
       <c r="H21">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I21">
         <v>2</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="J21:J23" si="9">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2026</v>
       </c>
       <c r="L21">
@@ -4780,275 +4758,279 @@
         <v>3</v>
       </c>
       <c r="M21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="G22">
+        <f t="shared" si="8"/>
         <v>2023</v>
       </c>
       <c r="H22">
-        <f>$D$5+$D$6</f>
-        <v>3</v>
+        <f>$D$6</f>
+        <v>2</v>
       </c>
       <c r="I22">
         <v>2</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22" si="7">ROUNDDOWN(G22+H22+I22*(1-J22),0)</f>
-        <v>2027</v>
+        <f t="shared" si="3"/>
+        <v>2026</v>
       </c>
       <c r="L22">
-        <f t="shared" ref="L22" si="8">K22-G22</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="G23">
-        <v>2020</v>
+        <f>$D$4+$D$5</f>
+        <v>2024</v>
       </c>
       <c r="H23">
-        <f>$D$5</f>
-        <v>2</v>
+        <f>$D$6+$D$7</f>
+        <v>3</v>
       </c>
       <c r="I23">
         <v>2</v>
       </c>
       <c r="J23">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="K23" si="10">ROUNDDOWN(G23+H23+I23*(1-J23),0)</f>
+        <v>2028</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ref="L23" si="11">K23-G23</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24">
+        <v>2020</v>
+      </c>
+      <c r="H24">
+        <f>$D$6</f>
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
         <v>0.5</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="2"/>
+      <c r="K24">
+        <f t="shared" si="3"/>
         <v>2023</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>6</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>5</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>2021</v>
       </c>
-      <c r="H24">
-        <f>$D$5</f>
+      <c r="H25">
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <v>3.5</v>
       </c>
-      <c r="J24">
-        <f t="shared" ref="J24:J25" si="9">$D$3</f>
+      <c r="J25">
+        <f t="shared" ref="J25:J26" si="12">$D$3</f>
         <v>0.25</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="2"/>
+      <c r="K25">
+        <f t="shared" si="3"/>
         <v>2025</v>
       </c>
-      <c r="L24">
+      <c r="L25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>154</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>67</v>
       </c>
-      <c r="G25">
+      <c r="G26">
+        <f t="shared" ref="G26" si="13">$D$4</f>
         <v>2023</v>
       </c>
-      <c r="H25">
-        <f>$D$5</f>
+      <c r="H26">
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>1</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="9"/>
+      <c r="J26">
+        <f t="shared" si="12"/>
         <v>0.25</v>
       </c>
-      <c r="K25">
-        <f>ROUNDDOWN(G25+H25+I25*(1-J25),0)</f>
+      <c r="K26">
+        <f>ROUNDDOWN(G26+H26+I26*(1-J26),0)</f>
         <v>2025</v>
       </c>
-      <c r="L25">
+      <c r="L26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M26" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26">
-        <v>2025</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <f>ROUNDDOWN(G26+H26+I26*(1-J26),0)</f>
-        <v>2028</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M26" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>25</v>
+        <v>155</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="H27">
-        <f t="shared" ref="H27:H36" si="10">$D$5</f>
         <v>2</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K27">
-        <f t="shared" si="2"/>
-        <v>2024</v>
+        <f>ROUNDDOWN(G27+H27+I27*(1-J27),0)</f>
+        <v>2028</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M27" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
         <v>23</v>
@@ -5057,466 +5039,470 @@
         <v>24</v>
       </c>
       <c r="G28">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H28">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I28">
         <v>2</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28:J30" si="11">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K28">
-        <f t="shared" si="2"/>
-        <v>2026</v>
+        <f t="shared" si="3"/>
+        <v>2024</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M28" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>73</v>
-      </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G29">
-        <v>2021</v>
+        <f t="shared" ref="G29" si="14">$D$4</f>
+        <v>2023</v>
       </c>
       <c r="H29">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J29">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="J29:J31" si="15">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2026</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" t="s">
-        <v>24</v>
-      </c>
       <c r="G30">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H30">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I30">
         <v>4</v>
       </c>
       <c r="J30">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.25</v>
       </c>
       <c r="K30">
-        <f t="shared" si="2"/>
-        <v>2028</v>
+        <f t="shared" si="3"/>
+        <v>2026</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M30" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G31">
-        <v>2018</v>
+        <f t="shared" ref="G31" si="16">$D$4</f>
+        <v>2023</v>
       </c>
       <c r="H31">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="I31" t="s">
-        <v>80</v>
-      </c>
-      <c r="J31" t="s">
-        <v>80</v>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="15"/>
+        <v>0.25</v>
       </c>
       <c r="K31">
-        <v>2020</v>
+        <f t="shared" si="3"/>
+        <v>2028</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32">
+        <v>2018</v>
+      </c>
+      <c r="H32">
+        <f>$D$6</f>
         <v>2</v>
       </c>
-      <c r="M31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" t="s">
-        <v>159</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32">
-        <v>2021</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="I32">
-        <v>4</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ref="J32:J36" si="12">$D$3</f>
-        <v>0.25</v>
+      <c r="I32" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" t="s">
+        <v>80</v>
       </c>
       <c r="K32">
-        <f t="shared" si="2"/>
-        <v>2026</v>
+        <v>2020</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="M32" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>16</v>
+        <v>159</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
       </c>
       <c r="G33">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H33">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I33">
         <v>4</v>
       </c>
       <c r="J33">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="J33:J37" si="17">$D$3</f>
         <v>0.25</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
-        <v>2028</v>
+        <f t="shared" si="3"/>
+        <v>2026</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M33" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
+        <v>160</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G34">
+        <f t="shared" ref="G34:G35" si="18">$D$4</f>
         <v>2023</v>
       </c>
       <c r="H34">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I34">
         <v>4</v>
       </c>
       <c r="J34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="K34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2028</v>
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="M34" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>87</v>
-      </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>89</v>
+        <v>161</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
       </c>
       <c r="G35">
-        <v>2021</v>
+        <f t="shared" si="18"/>
+        <v>2023</v>
       </c>
       <c r="H35">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="K35">
-        <f t="shared" si="2"/>
-        <v>2024</v>
+        <f t="shared" si="3"/>
+        <v>2028</v>
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" t="s">
-        <v>3</v>
+        <v>162</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
       </c>
       <c r="G36">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="H36">
-        <f t="shared" si="10"/>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>0.25</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
-        <v>2028</v>
+        <f t="shared" si="3"/>
+        <v>2024</v>
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" t="s">
-        <v>111</v>
-      </c>
-      <c r="F37" t="s">
-        <v>112</v>
-      </c>
       <c r="G37">
+        <f t="shared" ref="G37:G39" si="19">$D$4</f>
         <v>2023</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <f>$D$6</f>
+        <v>2</v>
       </c>
       <c r="I37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>0.25</v>
       </c>
       <c r="K37">
-        <f t="shared" si="2"/>
-        <v>2025</v>
+        <f t="shared" si="3"/>
+        <v>2028</v>
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M37" t="s">
-        <v>113</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
+        <v>164</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="G38">
+        <f t="shared" si="19"/>
         <v>2023</v>
       </c>
       <c r="H38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J38">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="2"/>
-        <v>2026</v>
+        <f t="shared" si="3"/>
+        <v>2025</v>
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M38" t="s">
-        <v>169</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="D39" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="F39" t="s">
-        <v>126</v>
+        <v>15</v>
       </c>
       <c r="G39">
-        <v>2024</v>
+        <f t="shared" si="19"/>
+        <v>2023</v>
       </c>
       <c r="H39">
-        <f>$D$5+$D$6</f>
         <v>3</v>
       </c>
       <c r="I39">
@@ -5526,26 +5512,29 @@
         <v>0.25</v>
       </c>
       <c r="K39">
-        <f t="shared" si="2"/>
-        <v>2027</v>
+        <f t="shared" si="3"/>
+        <v>2026</v>
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M39" t="s">
-        <v>136</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
         <v>122</v>
@@ -5554,10 +5543,11 @@
         <v>126</v>
       </c>
       <c r="G40">
-        <v>2025</v>
+        <f>$D$4+$D$5</f>
+        <v>2024</v>
       </c>
       <c r="H40">
-        <f t="shared" ref="H40:H41" si="13">$D$5+$D$6</f>
+        <f>$D$6+$D$7</f>
         <v>3</v>
       </c>
       <c r="I40">
@@ -5567,8 +5557,8 @@
         <v>0.25</v>
       </c>
       <c r="K40">
-        <f t="shared" si="2"/>
-        <v>2028</v>
+        <f t="shared" si="3"/>
+        <v>2027</v>
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
@@ -5580,25 +5570,26 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
         <v>126</v>
       </c>
       <c r="G41">
-        <v>2026</v>
+        <f>$D$4+$D$5</f>
+        <v>2024</v>
       </c>
       <c r="H41">
-        <f t="shared" si="13"/>
+        <f>$D$6+$D$7</f>
         <v>3</v>
       </c>
       <c r="I41">
@@ -5608,8 +5599,8 @@
         <v>0.25</v>
       </c>
       <c r="K41">
-        <f t="shared" si="2"/>
-        <v>2029</v>
+        <f t="shared" si="3"/>
+        <v>2027</v>
       </c>
       <c r="L41">
         <f t="shared" si="1"/>
@@ -5621,26 +5612,27 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>129</v>
       </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="F42" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="G42">
-        <v>2031</v>
+        <f>$D$4+$D$5</f>
+        <v>2024</v>
       </c>
       <c r="H42">
-        <f>$D$6</f>
-        <v>1</v>
+        <f>$D$6+$D$7</f>
+        <v>3</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -5649,12 +5641,12 @@
         <v>0.25</v>
       </c>
       <c r="K42">
-        <f t="shared" ref="K42:K43" si="14">ROUNDDOWN(G42+H42+I42*(1-J42),0)</f>
-        <v>2032</v>
+        <f t="shared" si="3"/>
+        <v>2027</v>
       </c>
       <c r="L42">
-        <f t="shared" ref="L42:L43" si="15">K42-G42</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="M42" t="s">
         <v>136</v>
@@ -5662,25 +5654,25 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F43" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G43">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:H44" si="16">$D$6</f>
+        <f>$D$7</f>
         <v>1</v>
       </c>
       <c r="I43">
@@ -5690,11 +5682,11 @@
         <v>0.25</v>
       </c>
       <c r="K43">
-        <f t="shared" si="14"/>
-        <v>2031</v>
+        <f t="shared" ref="K43:K44" si="20">ROUNDDOWN(G43+H43+I43*(1-J43),0)</f>
+        <v>2032</v>
       </c>
       <c r="L43">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="L43:L44" si="21">K43-G43</f>
         <v>1</v>
       </c>
       <c r="M43" t="s">
@@ -5703,25 +5695,25 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G44">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="H44">
-        <f t="shared" si="16"/>
+        <f>$D$7</f>
         <v>1</v>
       </c>
       <c r="I44">
@@ -5731,11 +5723,11 @@
         <v>0.25</v>
       </c>
       <c r="K44">
-        <f t="shared" ref="K44" si="17">ROUNDDOWN(G44+H44+I44*(1-J44),0)</f>
-        <v>2030</v>
+        <f t="shared" si="20"/>
+        <v>2031</v>
       </c>
       <c r="L44">
-        <f t="shared" ref="L44" si="18">K44-G44</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="M44" t="s">
@@ -5743,70 +5735,71 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>118</v>
-      </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="E45" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="G45">
-        <v>2024</v>
+        <v>2029</v>
       </c>
       <c r="H45">
-        <f>$D$5</f>
-        <v>2</v>
+        <f>$D$7</f>
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45">
         <v>0.25</v>
       </c>
       <c r="K45">
-        <f t="shared" si="2"/>
-        <v>2027</v>
+        <f t="shared" ref="K45" si="22">ROUNDDOWN(G45+H45+I45*(1-J45),0)</f>
+        <v>2030</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" ref="L45" si="23">K45-G45</f>
+        <v>1</v>
       </c>
       <c r="M45" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="F46" t="s">
         <v>67</v>
       </c>
       <c r="G46">
+        <f>$D$4+$D$5</f>
         <v>2024</v>
       </c>
       <c r="H46">
-        <f>$D$5</f>
+        <f>$D$6</f>
         <v>2</v>
       </c>
       <c r="I46">
@@ -5816,7 +5809,7 @@
         <v>0.25</v>
       </c>
       <c r="K46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2027</v>
       </c>
       <c r="L46">
@@ -5827,38 +5820,71 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47">
+        <v>2024</v>
+      </c>
+      <c r="H47">
+        <f>$D$6</f>
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>0.25</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="3"/>
+        <v>2027</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H51" s="6" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H52" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="H52" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I52" s="8">
-        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H53" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I53" s="8">
         <v>4</v>
-      </c>
-      <c r="I53" s="8">
-        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H54" s="7" t="s">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="I54" s="8">
         <v>1</v>
@@ -5866,39 +5892,39 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H55" s="7" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="I55" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H56" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I56" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H57" s="7" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I57" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H58" s="7" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="I58" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H59" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="I59" s="8">
         <v>2</v>
@@ -5906,23 +5932,23 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H60" s="7" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="I60" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H61" s="7" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="I61" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H62" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I62" s="8">
         <v>4</v>
@@ -5930,31 +5956,31 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H63" s="7" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="I63" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="H64" s="7" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="I64" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H65" s="7" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="I65" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H66" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I66" s="8">
         <v>2</v>
@@ -5962,7 +5988,7 @@
     </row>
     <row r="67" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H67" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I67" s="8">
         <v>2</v>
@@ -5970,30 +5996,38 @@
     </row>
     <row r="68" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H68" s="7" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="I68" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H69" s="7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I69" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H70" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="I70" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.35">
+      <c r="H71" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="I70" s="8">
+      <c r="I71" s="8">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E9:E46" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
+  <autoFilter ref="E10:E47" xr:uid="{57F1FF48-4396-4FE3-ABD9-234FB66F60F4}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated port investment schedule to included floating marshaling ports
</commit_message>
<xml_diff>
--- a/fabrication_ports/ports_scenario_min.xlsx
+++ b/fabrication_ports/ports_scenario_min.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\fabrication_ports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8168957-1A85-4B46-AEB9-EBC6775D6EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62F5D24-C993-4FAA-B745-90E7106E4E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="9" r:id="rId1"/>
@@ -4200,7 +4200,7 @@
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="B29" sqref="A29:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>